<commit_message>
fixed page 4 fonts and arrangements
</commit_message>
<xml_diff>
--- a/static/Certificate_Page4.xlsx
+++ b/static/Certificate_Page4.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,7 +27,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
       <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12"/>
     </font>
     <font>
       <color rgb="0057C4E5"/>
@@ -35,6 +41,10 @@
     <font>
       <b val="1"/>
       <sz val="23"/>
+    </font>
+    <font>
+      <name val="Arial Black"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,24 +67,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -155,12 +167,12 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>1</col>
       <colOff>0</colOff>
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1619250" cy="952500"/>
+    <ext cx="1000125" cy="1000125"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -470,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,231 +499,424 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Republic of the Philippines</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Bicol University</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n"/>
       <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>OFFICE OF THE UNIVERSITY REGISTRAR</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
       <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>Legazpi City</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n"/>
-      <c r="H4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>Tel. No (052) 820-6809</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
       <c r="F5" s="1" t="n"/>
-      <c r="G5" s="1" t="n"/>
-      <c r="H5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>E-mail Add: bu_uro@yahoo.com</t>
         </is>
       </c>
-      <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="n"/>
-      <c r="G6" s="1" t="n"/>
-      <c r="H6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>ISO 9001:2008</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Certificate No.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>TUV100 05 1782</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>C E R T I F I C A T I O N</t>
         </is>
       </c>
     </row>
+    <row r="13"/>
     <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="6" t="inlineStr">
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>TO WHOM IT MAY CONCERN:</t>
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
+      <c r="D16" s="6" t="n"/>
+      <c r="E16" s="6" t="n"/>
+      <c r="F16" s="6" t="n"/>
+      <c r="G16" s="6" t="n"/>
+      <c r="H16" s="6" t="n"/>
+      <c r="I16" s="6" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n"/>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="6" t="n"/>
+      <c r="E17" s="6" t="n"/>
+      <c r="F17" s="6" t="n"/>
+      <c r="G17" s="6" t="n"/>
+      <c r="H17" s="6" t="n"/>
+      <c r="I17" s="6" t="n"/>
+    </row>
     <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">         This is to certify that Ms. FRANCIA Q. LLABAN has graduated with the degree</t>
-        </is>
-      </c>
+      <c r="A18" s="6" t="n"/>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         This is to certify that Ms. FRANCIA Q. LLABAN has graduated with the degree of</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="n"/>
+      <c r="H18" s="6" t="n"/>
+      <c r="I18" s="6" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>of Bachelor of Science in Industrial Education (BSIE) major in Food Technology,</t>
-        </is>
-      </c>
+      <c r="A19" s="6" t="n"/>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>Bachelor of Science in Industrial Education (BSIE) major in Food Technology, Cum Laude</t>
+        </is>
+      </c>
+      <c r="G19" s="6" t="n"/>
+      <c r="H19" s="6" t="n"/>
+      <c r="I19" s="6" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Cum Laude on April 03, 1997 per Resolution No. 1, s. 1997 of the Board of Regents,</t>
-        </is>
-      </c>
+      <c r="A20" s="6" t="n"/>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> on April 03, 1997 per Resolution No. 1, s. 1997 of the Board of Regents, Bicol University.</t>
+        </is>
+      </c>
+      <c r="G20" s="6" t="n"/>
+      <c r="H20" s="6" t="n"/>
+      <c r="I20" s="6" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Bicol University.</t>
-        </is>
-      </c>
+      <c r="A21" s="6" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="6" t="n"/>
+      <c r="E21" s="6" t="n"/>
+      <c r="F21" s="6" t="n"/>
+      <c r="G21" s="6" t="n"/>
+      <c r="H21" s="6" t="n"/>
+      <c r="I21" s="6" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n"/>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         It is further certified that she is of good moral character and has never been subjected to </t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="6" t="n"/>
+      <c r="E22" s="6" t="n"/>
+      <c r="F22" s="6" t="n"/>
+      <c r="G22" s="6" t="n"/>
+      <c r="H22" s="6" t="n"/>
+      <c r="I22" s="6" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">         It is further certified that she is of good moral character and has never been</t>
-        </is>
-      </c>
+      <c r="A23" s="6" t="n"/>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>any disciplinary action during her entire stay in this University.</t>
+        </is>
+      </c>
+      <c r="G23" s="6" t="n"/>
+      <c r="H23" s="6" t="n"/>
+      <c r="I23" s="6" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>subjected to any disciplinary action during her entire stay in this University.</t>
-        </is>
-      </c>
+      <c r="A24" s="6" t="n"/>
+      <c r="B24" s="6" t="n"/>
+      <c r="G24" s="6" t="n"/>
+      <c r="H24" s="6" t="n"/>
+      <c r="I24" s="6" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n"/>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         Issued this 21st day of June, 2010 upon the request of Ms. Llaban for reference purposes.</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="6" t="n"/>
+      <c r="E25" s="6" t="n"/>
+      <c r="F25" s="6" t="n"/>
+      <c r="G25" s="6" t="n"/>
+      <c r="H25" s="6" t="n"/>
+      <c r="I25" s="6" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">         Issued this 21st day of June, 2010 upon the request of Ms. Llaban for reference</t>
-        </is>
-      </c>
+      <c r="A26" s="6" t="n"/>
+      <c r="B26" s="6" t="n"/>
+      <c r="G26" s="6" t="n"/>
+      <c r="H26" s="6" t="n"/>
+      <c r="I26" s="6" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>purposes.</t>
-        </is>
-      </c>
+      <c r="A27" s="6" t="n"/>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="6" t="n"/>
+      <c r="E27" s="6" t="n"/>
+      <c r="F27" s="6" t="n"/>
+      <c r="G27" s="6" t="n"/>
+      <c r="H27" s="6" t="n"/>
+      <c r="I27" s="6" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n"/>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
+      <c r="D28" s="6" t="n"/>
+      <c r="E28" s="6" t="n"/>
+      <c r="F28" s="6" t="n"/>
+      <c r="G28" s="6" t="n"/>
+      <c r="H28" s="6" t="n"/>
+      <c r="I28" s="6" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n"/>
+      <c r="B29" s="6" t="n"/>
+      <c r="C29" s="6" t="n"/>
+      <c r="D29" s="6" t="n"/>
+      <c r="E29" s="6" t="n"/>
+      <c r="F29" s="6" t="n"/>
+      <c r="G29" s="6" t="n"/>
+      <c r="H29" s="6" t="n"/>
+      <c r="I29" s="6" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n"/>
+      <c r="B30" s="6" t="n"/>
+      <c r="C30" s="6" t="n"/>
+      <c r="D30" s="6" t="n"/>
+      <c r="E30" s="6" t="n"/>
+      <c r="F30" s="6" t="n"/>
+      <c r="G30" s="6" t="n"/>
+      <c r="H30" s="6" t="n"/>
+      <c r="I30" s="6" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n"/>
+      <c r="B31" s="6" t="n"/>
+      <c r="C31" s="6" t="n"/>
+      <c r="D31" s="6" t="n"/>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>CORAZON N. BAZAR</t>
+        </is>
+      </c>
+      <c r="G31" s="6" t="n"/>
+      <c r="H31" s="6" t="n"/>
+      <c r="I31" s="6" t="n"/>
     </row>
     <row r="32">
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Corazon N. Bazar</t>
-        </is>
-      </c>
+      <c r="A32" s="6" t="n"/>
+      <c r="B32" s="6" t="n"/>
+      <c r="C32" s="6" t="n"/>
+      <c r="D32" s="6" t="n"/>
+      <c r="E32" s="6" t="n"/>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>University Registrar</t>
+        </is>
+      </c>
+      <c r="G32" s="6" t="n"/>
+      <c r="H32" s="6" t="n"/>
+      <c r="I32" s="6" t="n"/>
     </row>
     <row r="33">
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>University Registrar</t>
-        </is>
-      </c>
+      <c r="A33" s="6" t="n"/>
+      <c r="B33" s="6" t="n"/>
+      <c r="C33" s="6" t="n"/>
+      <c r="D33" s="6" t="n"/>
+      <c r="E33" s="6" t="n"/>
+      <c r="F33" s="6" t="n"/>
+      <c r="G33" s="6" t="n"/>
+      <c r="H33" s="6" t="n"/>
+      <c r="I33" s="6" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n"/>
+      <c r="B34" s="6" t="n"/>
+      <c r="C34" s="6" t="n"/>
+      <c r="D34" s="6" t="n"/>
+      <c r="E34" s="6" t="n"/>
+      <c r="F34" s="6" t="n"/>
+      <c r="G34" s="6" t="n"/>
+      <c r="H34" s="6" t="n"/>
+      <c r="I34" s="6" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n"/>
+      <c r="B35" s="6" t="n"/>
+      <c r="C35" s="6" t="n"/>
+      <c r="D35" s="6" t="n"/>
+      <c r="E35" s="6" t="n"/>
+      <c r="F35" s="6" t="n"/>
+      <c r="G35" s="6" t="n"/>
+      <c r="H35" s="6" t="n"/>
+      <c r="I35" s="6" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n"/>
+      <c r="B36" s="6" t="n"/>
+      <c r="C36" s="6" t="n"/>
+      <c r="D36" s="6" t="n"/>
+      <c r="E36" s="6" t="n"/>
+      <c r="F36" s="6" t="n"/>
+      <c r="G36" s="6" t="n"/>
+      <c r="H36" s="6" t="n"/>
+      <c r="I36" s="6" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n"/>
+      <c r="B37" s="8" t="inlineStr">
+        <is>
+          <t>BU-F-UREG-54</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="n"/>
+      <c r="D37" s="6" t="n"/>
+      <c r="E37" s="6" t="n"/>
+      <c r="F37" s="8" t="inlineStr">
+        <is>
+          <t>Revision: 1</t>
+        </is>
+      </c>
+      <c r="G37" s="6" t="n"/>
+      <c r="H37" s="6" t="n"/>
+      <c r="I37" s="6" t="n"/>
     </row>
     <row r="38">
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>BU-F-UREG-54</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Revision: 1</t>
-        </is>
-      </c>
+      <c r="A38" s="6" t="n"/>
+      <c r="B38" s="8" t="inlineStr">
+        <is>
+          <t>Effectivity Date: Mar. 9,2011</t>
+        </is>
+      </c>
+      <c r="C38" s="6" t="n"/>
+      <c r="D38" s="6" t="n"/>
+      <c r="E38" s="6" t="n"/>
+      <c r="F38" s="6" t="n"/>
+      <c r="G38" s="6" t="n"/>
+      <c r="H38" s="6" t="n"/>
+      <c r="I38" s="6" t="n"/>
     </row>
     <row r="39">
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Effectivity Date: Mar. 9,2011</t>
-        </is>
-      </c>
+      <c r="A39" s="6" t="n"/>
+      <c r="B39" s="6" t="n"/>
+      <c r="C39" s="6" t="n"/>
+      <c r="D39" s="6" t="n"/>
+      <c r="E39" s="6" t="n"/>
+      <c r="F39" s="6" t="n"/>
+      <c r="G39" s="6" t="n"/>
+      <c r="H39" s="6" t="n"/>
+      <c r="I39" s="6" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n"/>
+      <c r="B40" s="6" t="n"/>
+      <c r="C40" s="6" t="n"/>
+      <c r="D40" s="6" t="n"/>
+      <c r="E40" s="6" t="n"/>
+      <c r="F40" s="6" t="n"/>
+      <c r="G40" s="6" t="n"/>
+      <c r="H40" s="6" t="n"/>
+      <c r="I40" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
+  <mergeCells count="13">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A12:F13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B26:F26"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperHeight="13in" paperWidth="8.5in"/>

</xml_diff>